<commit_message>
added new pivots to refresh code
all pivot tables on the main page now refresh when new data is pulled from the refresh button
</commit_message>
<xml_diff>
--- a/_Config-OTR-RTS.xlsx
+++ b/_Config-OTR-RTS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20404"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garbosz\Desktop\keep files\OTR Bridge Tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garbosz\Documents\GitHub\RTS WASH TOOLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25CDA1AC-6640-44C3-BC2F-899B79EB8FB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BD3099-0298-4B02-8A00-9F31CEBA9D47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,9 +75,6 @@
     <t>Seven 4 Logistics</t>
   </si>
   <si>
-    <t>mcgarrybecca02@gmail.com; obrien.gene100@gmail.com;crystalleparent@gmail.com</t>
-  </si>
-  <si>
     <t>SVLC</t>
   </si>
   <si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>dbo6-otr-team@amazon.com</t>
+  </si>
+  <si>
+    <t>mcgarrybecca02@gmail.com; obrien.gene100@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -446,8 +446,8 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B18:B19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -516,46 +516,46 @@
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
         <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -565,28 +565,13 @@
     <hyperlink ref="B3" r:id="rId3" xr:uid="{FE9C2E49-2C90-41AB-9BB9-F1D29F9F892A}"/>
     <hyperlink ref="B7" r:id="rId4" display=" jerryjtulsa@yahoo.com; ddumas@soonertransportation.net; adiaz@soonertransportation.net;  sstewart@soonertransportation.net;lacevedo@soonertransportation.net;lacevedo@soonertransportation.net " xr:uid="{F52691CB-254D-4AEE-AE64-BC942D0B9FDF}"/>
     <hyperlink ref="B5" r:id="rId5" xr:uid="{1BFF2D29-060D-41F9-825C-A15C79966020}"/>
-    <hyperlink ref="B6" r:id="rId6" xr:uid="{98B3996F-6CB5-4D0B-9536-9DBC26821145}"/>
+    <hyperlink ref="B6" r:id="rId6" display="mcgarrybecca02@gmail.com; obrien.gene100@gmail.com;crystalleparent@gmail.com" xr:uid="{98B3996F-6CB5-4D0B-9536-9DBC26821145}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010009E7C346E1BF4E4A88387C42754D82E8" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="396691cd37cd27f08540a1fab9de27af">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="959c0417-1dec-4a77-b0f6-6a2944d93699" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="37a9dce94ad5fda67456b4f26bfbe21d" ns2:_="">
     <xsd:import namespace="959c0417-1dec-4a77-b0f6-6a2944d93699"/>
@@ -726,31 +711,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC96791E-D1A0-4EC5-ACBC-48B21EBF1C43}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="959c0417-1dec-4a77-b0f6-6a2944d93699"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB80572-BC99-40A6-AC26-9739E934703E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FE2495E-21E8-4E31-BFE0-93D0A2FDC5A9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -766,4 +742,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB80572-BC99-40A6-AC26-9739E934703E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC96791E-D1A0-4EC5-ACBC-48B21EBF1C43}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="959c0417-1dec-4a77-b0f6-6a2944d93699"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>